<commit_message>
correction of the name of the variable amount in the database
</commit_message>
<xml_diff>
--- a/src/seed/books.xlsx
+++ b/src/seed/books.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Especialización Desarrollo de Software\1er Semestre\Módulo 2\bookease\src\seed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E5B3EA-D0A1-49F6-B76B-C0243DD33F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E12DF82-411B-4EBC-A0B3-C9ABD1D881F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1354,10 +1354,13 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="66.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1733,7 +1736,7 @@
         <v>301</v>
       </c>
       <c r="E19" s="2">
-        <v>84.94</v>
+        <v>59.39</v>
       </c>
       <c r="F19">
         <v>26</v>
@@ -1913,7 +1916,7 @@
         <v>302</v>
       </c>
       <c r="E28" s="2">
-        <v>22.9</v>
+        <v>59.39</v>
       </c>
       <c r="F28">
         <v>50</v>
@@ -2073,7 +2076,7 @@
         <v>304</v>
       </c>
       <c r="E36" s="2">
-        <v>11.69</v>
+        <v>59.39</v>
       </c>
       <c r="F36">
         <v>3</v>
@@ -2133,7 +2136,7 @@
         <v>304</v>
       </c>
       <c r="E39" s="2">
-        <v>65.52</v>
+        <v>59.39</v>
       </c>
       <c r="F39">
         <v>12</v>
@@ -2333,7 +2336,7 @@
         <v>299</v>
       </c>
       <c r="E49" s="2">
-        <v>21.6</v>
+        <v>59.39</v>
       </c>
       <c r="F49">
         <v>4</v>

</xml_diff>